<commit_message>
making all summary stats related fields optional.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.4.xlsx
+++ b/schema_definitions/template_schema_v1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDE7D59-4571-D84D-A422-C7CE81EA872D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A139DBCB-2D17-334C-A88A-7701EB5B1867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="2280" windowWidth="48040" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="180">
   <si>
     <t>NAME</t>
   </si>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1528,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>24</v>
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>24</v>
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>24</v>
@@ -1627,7 +1627,10 @@
         <v>53</v>
       </c>
       <c r="M19" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="O19" s="5" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
Minor changes in the schema
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.4.xlsx
+++ b/schema_definitions/template_schema_v1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F86926B-70E8-8046-AFDB-1F4251558852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B581895E-3373-3845-A0BE-42C9A3DE58A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="32440" yWindow="-1060" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
   <si>
     <t>NAME</t>
   </si>
@@ -544,9 +544,6 @@
     <t>Path or URL pointing to the file containing additional information for the provided summary statistics file</t>
   </si>
   <si>
-    <t>^[actgACTG?-]*$</t>
-  </si>
-  <si>
     <t>Aboriginal Australian|African American or Afro-Caribbean|African unspecified|Asian unspecified|Central Asian|Circumpolar peoples|East Asian|European|Greater Middle Eastern (Middle Eastern, North African or Persian)|Hispanic or Latin American|Native American|NR|Oceanian|Other|Other admixed ancestry|South Asian|South East Asian|Sub-Saharan African</t>
   </si>
   <si>
@@ -578,13 +575,19 @@
   </si>
   <si>
     <t>Cohort specific identifier(s) issued to this research study</t>
+  </si>
+  <si>
+    <t>Illumina|Perlegen|Affymetrix</t>
+  </si>
+  <si>
+    <t>^[ACTG?-]*$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -639,6 +642,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -661,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -673,6 +682,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="M1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1049,10 +1059,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>9</v>
@@ -1152,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>26</v>
@@ -1190,7 +1200,10 @@
         <v>1</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1249,7 +1262,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>35</v>
@@ -1441,7 +1454,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1508,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1630,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -1641,7 +1654,7 @@
         <v>149</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20" s="5" t="b">
         <v>1</v>
@@ -1668,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -1676,7 +1689,7 @@
         <v>151</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="5" t="b">
         <v>1</v>
@@ -1703,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1717,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1777,10 +1790,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>9</v>
@@ -1991,7 +2004,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>125</v>
@@ -2023,7 +2036,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>122</v>
@@ -2309,10 +2322,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>9</v>
@@ -2370,7 +2383,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>99</v>
@@ -2535,10 +2548,10 @@
         <v>1</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2631,7 +2644,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3692,10 +3705,10 @@
         <v>8</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>9</v>
@@ -3778,7 +3791,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>68</v>
@@ -3810,7 +3823,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Changing p-value field to numeric
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.4.xlsx
+++ b/schema_definitions/template_schema_v1.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B581895E-3373-3845-A0BE-42C9A3DE58A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38C1E6E-EA93-6B43-8F7C-E27DED0C3E78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32440" yWindow="-1060" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,7 +1906,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="J5" s="5">
         <v>0</v>

</xml_diff>